<commit_message>
sprint 17 (changes suggested by ronak in mail)
</commit_message>
<xml_diff>
--- a/media/reports/All_Input.xlsx
+++ b/media/reports/All_Input.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Reports" sheetId="1" state="visible" r:id="rId1"/>
@@ -68,17 +68,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -455,7 +455,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>akhil</t>
         </is>
       </c>
     </row>
@@ -467,7 +467,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>org name</t>
+          <t>rk indusreis</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2020-07-29</t>
+          <t>2020-10-05</t>
         </is>
       </c>
     </row>
@@ -507,7 +507,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2020-07-16</t>
+          <t>01-10-2020</t>
         </is>
       </c>
     </row>
@@ -519,7 +519,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2020-07-31</t>
+          <t>31-10-2020</t>
         </is>
       </c>
     </row>
@@ -553,12 +553,12 @@
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>2020-07-29</t>
+          <t>2020-10-05</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>register</t>
+          <t>gst report test</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>120</v>
+        <v>48.14</v>
       </c>
     </row>
     <row r="11">
@@ -587,6 +587,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>